<commit_message>
Update with Q1 2025 construction spending
</commit_message>
<xml_diff>
--- a/data/BEA/bea_const_price_indices.xlsx
+++ b/data/BEA/bea_const_price_indices.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="114">
   <si>
     <t xml:space="preserve">Table 5.3.4. Price Indexes for Private Fixed Investment by Type</t>
   </si>
@@ -23,7 +23,7 @@
     <t xml:space="preserve">Bureau of Economic Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">Last Revised on: March 27, 2025 - Next Release Date April 30, 2025</t>
+    <t xml:space="preserve">Last Revised on: April 30, 2025 - Next Release Date May 29, 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Line</t>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
@@ -552,7 +555,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:EA49"/>
+  <dimension ref="A1:EB49"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
@@ -688,6 +691,7 @@
     <col min="128" max="128" width="7.95" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="129" max="129" width="7.95" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="130" max="130" width="7.95" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="131" max="131" width="7.800000000000001" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -910,401 +914,407 @@
       <c r="DX6" s="1"/>
       <c r="DY6" s="1"/>
       <c r="DZ6" s="1"/>
+      <c r="EA6" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="1" t="s">
+      <c r="V7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="X7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AG7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AE7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AK7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AI7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
+      <c r="AL7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AN7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AO7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AM7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN7" s="1" t="s">
+      <c r="AP7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO7" s="1" t="s">
+      <c r="AR7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP7" s="1" t="s">
+      <c r="AS7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AT7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AV7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AT7" s="1" t="s">
+      <c r="AW7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AV7" s="1" t="s">
+      <c r="AX7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AW7" s="1" t="s">
+      <c r="AZ7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AX7" s="1" t="s">
+      <c r="BA7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AY7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ7" s="1" t="s">
+      <c r="BB7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BA7" s="1" t="s">
+      <c r="BD7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BB7" s="1" t="s">
+      <c r="BE7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BC7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BD7" s="1" t="s">
+      <c r="BF7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BG7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BE7" s="1" t="s">
+      <c r="BH7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BF7" s="1" t="s">
+      <c r="BI7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BG7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BH7" s="1" t="s">
+      <c r="BJ7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BK7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BI7" s="1" t="s">
+      <c r="BL7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BJ7" s="1" t="s">
+      <c r="BM7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BK7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BL7" s="1" t="s">
+      <c r="BN7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BO7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BM7" s="1" t="s">
+      <c r="BP7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BN7" s="1" t="s">
+      <c r="BQ7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BO7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BP7" s="1" t="s">
+      <c r="BR7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BS7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BQ7" s="1" t="s">
+      <c r="BT7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BR7" s="1" t="s">
+      <c r="BU7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BS7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BT7" s="1" t="s">
+      <c r="BV7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BW7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BU7" s="1" t="s">
+      <c r="BX7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BV7" s="1" t="s">
+      <c r="BY7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="BW7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BX7" s="1" t="s">
+      <c r="BZ7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CA7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BY7" s="1" t="s">
+      <c r="CB7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BZ7" s="1" t="s">
+      <c r="CC7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CA7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CB7" s="1" t="s">
+      <c r="CD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CE7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CC7" s="1" t="s">
+      <c r="CF7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CD7" s="1" t="s">
+      <c r="CG7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CE7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CF7" s="1" t="s">
+      <c r="CH7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CI7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CG7" s="1" t="s">
+      <c r="CJ7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CH7" s="1" t="s">
+      <c r="CK7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CI7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CJ7" s="1" t="s">
+      <c r="CL7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CM7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CK7" s="1" t="s">
+      <c r="CN7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CL7" s="1" t="s">
+      <c r="CO7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CM7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CN7" s="1" t="s">
+      <c r="CP7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CQ7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CO7" s="1" t="s">
+      <c r="CR7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CP7" s="1" t="s">
+      <c r="CS7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CQ7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CR7" s="1" t="s">
+      <c r="CT7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CU7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CS7" s="1" t="s">
+      <c r="CV7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CT7" s="1" t="s">
+      <c r="CW7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CU7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CV7" s="1" t="s">
+      <c r="CX7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CY7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="CW7" s="1" t="s">
+      <c r="CZ7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CX7" s="1" t="s">
+      <c r="DA7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CY7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CZ7" s="1" t="s">
+      <c r="DB7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DC7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DA7" s="1" t="s">
+      <c r="DD7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DB7" s="1" t="s">
+      <c r="DE7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="DC7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DD7" s="1" t="s">
+      <c r="DF7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DG7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DE7" s="1" t="s">
+      <c r="DH7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DF7" s="1" t="s">
+      <c r="DI7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="DG7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DH7" s="1" t="s">
+      <c r="DJ7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DK7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DI7" s="1" t="s">
+      <c r="DL7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DJ7" s="1" t="s">
+      <c r="DM7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="DK7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DL7" s="1" t="s">
+      <c r="DN7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DO7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DM7" s="1" t="s">
+      <c r="DP7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DN7" s="1" t="s">
+      <c r="DQ7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="DO7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DP7" s="1" t="s">
+      <c r="DR7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DS7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DQ7" s="1" t="s">
+      <c r="DT7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DR7" s="1" t="s">
+      <c r="DU7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="DS7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DT7" s="1" t="s">
+      <c r="DV7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DW7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="DU7" s="1" t="s">
+      <c r="DX7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="DV7" s="1" t="s">
+      <c r="DY7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="DW7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DX7" s="1" t="s">
+      <c r="DZ7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="EA7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="DY7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="DZ7" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4">
         <v>78.549</v>
@@ -1689,14 +1699,17 @@
       </c>
       <c r="DZ8" s="4">
         <v>123.666</v>
+      </c>
+      <c r="EA8" s="4">
+        <v>124.041</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4">
         <v>93.399</v>
@@ -2081,14 +2094,17 @@
       </c>
       <c r="DZ9" s="4">
         <v>115.98</v>
+      </c>
+      <c r="EA9" s="4">
+        <v>116.109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4">
         <v>38.524</v>
@@ -2473,14 +2489,17 @@
       </c>
       <c r="DZ10" s="4">
         <v>135.041</v>
+      </c>
+      <c r="EA10" s="4">
+        <v>135.419</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0">
         <v>44.701</v>
@@ -2865,14 +2884,17 @@
       </c>
       <c r="DZ11" s="0">
         <v>156.951</v>
+      </c>
+      <c r="EA11" s="0">
+        <v>158.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="0">
         <v>46.035</v>
@@ -3257,14 +3279,17 @@
       </c>
       <c r="DZ12" s="0">
         <v>156.648</v>
+      </c>
+      <c r="EA12" s="0">
+        <v>157.933</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0">
         <v>50.367</v>
@@ -3649,14 +3674,17 @@
       </c>
       <c r="DZ13" s="0">
         <v>121.064</v>
+      </c>
+      <c r="EA13" s="0">
+        <v>120.701</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0">
         <v>14.278</v>
@@ -4041,14 +4069,17 @@
       </c>
       <c r="DZ14" s="0">
         <v>90.835</v>
+      </c>
+      <c r="EA14" s="0">
+        <v>89.18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" s="0">
         <v>48.198</v>
@@ -4433,14 +4464,17 @@
       </c>
       <c r="DZ15" s="0">
         <v>136.7</v>
+      </c>
+      <c r="EA15" s="0">
+        <v>137.472</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4">
         <v>140.344</v>
@@ -4825,14 +4859,17 @@
       </c>
       <c r="DZ16" s="4">
         <v>114.017</v>
+      </c>
+      <c r="EA16" s="4">
+        <v>114.18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" s="0">
         <v>488.05</v>
@@ -5217,14 +5254,17 @@
       </c>
       <c r="DZ17" s="0">
         <v>97.603</v>
+      </c>
+      <c r="EA17" s="0">
+        <v>97.834</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="0">
         <v>1547.222</v>
@@ -5609,14 +5649,17 @@
       </c>
       <c r="DZ18" s="0">
         <v>102.603</v>
+      </c>
+      <c r="EA18" s="0">
+        <v>102.902</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" s="0">
         <v>259.3</v>
@@ -6001,14 +6044,17 @@
       </c>
       <c r="DZ19" s="0">
         <v>95.619</v>
+      </c>
+      <c r="EA19" s="0">
+        <v>95.815</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="0">
         <v>69.092</v>
@@ -6393,14 +6439,17 @@
       </c>
       <c r="DZ20" s="0">
         <v>126.089</v>
+      </c>
+      <c r="EA20" s="0">
+        <v>126.909</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" s="0">
         <v>72.988</v>
@@ -6785,14 +6834,17 @@
       </c>
       <c r="DZ21" s="0">
         <v>114.777</v>
+      </c>
+      <c r="EA21" s="0">
+        <v>114.103</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="0">
         <v>68.72</v>
@@ -7177,14 +7229,17 @@
       </c>
       <c r="DZ22" s="0">
         <v>130.255</v>
+      </c>
+      <c r="EA22" s="0">
+        <v>130.632</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="4">
         <v>89.99</v>
@@ -7569,14 +7624,17 @@
       </c>
       <c r="DZ23" s="4">
         <v>109.033</v>
+      </c>
+      <c r="EA23" s="4">
+        <v>109.021</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="0">
         <v>158.199</v>
@@ -7961,14 +8019,17 @@
       </c>
       <c r="DZ24" s="0">
         <v>92.241</v>
+      </c>
+      <c r="EA24" s="0">
+        <v>91.092</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="0">
         <v>62.492</v>
@@ -8353,14 +8414,17 @@
       </c>
       <c r="DZ25" s="0">
         <v>123.186</v>
+      </c>
+      <c r="EA25" s="0">
+        <v>124.314</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" s="0">
         <v>76.36</v>
@@ -8745,14 +8809,17 @@
       </c>
       <c r="DZ26" s="0">
         <v>124.407</v>
+      </c>
+      <c r="EA26" s="0">
+        <v>125.879</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4">
         <v>48.021</v>
@@ -9137,14 +9204,17 @@
       </c>
       <c r="DZ27" s="4">
         <v>150.781</v>
+      </c>
+      <c r="EA27" s="4">
+        <v>152.23</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" s="4">
         <v>47.15</v>
@@ -9529,14 +9599,17 @@
       </c>
       <c r="DZ28" s="4">
         <v>151.644</v>
+      </c>
+      <c r="EA28" s="4">
+        <v>153.192</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C29" s="0">
         <v>43.959</v>
@@ -9921,14 +9994,17 @@
       </c>
       <c r="DZ29" s="0">
         <v>149.926</v>
+      </c>
+      <c r="EA29" s="0">
+        <v>151.963</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="0">
         <v>45.904</v>
@@ -10313,14 +10389,17 @@
       </c>
       <c r="DZ30" s="0">
         <v>153.676</v>
+      </c>
+      <c r="EA30" s="0">
+        <v>155.859</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31" s="0">
         <v>37.052</v>
@@ -10705,14 +10784,17 @@
       </c>
       <c r="DZ31" s="0">
         <v>136.026</v>
+      </c>
+      <c r="EA31" s="0">
+        <v>137.574</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C32" s="0">
         <v>51.216</v>
@@ -11097,14 +11179,17 @@
       </c>
       <c r="DZ32" s="0">
         <v>152.983</v>
+      </c>
+      <c r="EA32" s="0">
+        <v>154.092</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4">
         <v>130.053</v>
@@ -11489,6 +11574,9 @@
       </c>
       <c r="DZ33" s="4">
         <v>111.445</v>
+      </c>
+      <c r="EA33" s="4">
+        <v>108.879</v>
       </c>
     </row>
     <row r="34">
@@ -11496,7 +11584,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>5</v>
@@ -11880,15 +11968,18 @@
         <v>5</v>
       </c>
       <c r="DZ34" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="EA34" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35" s="0">
         <v>43.741</v>
@@ -12273,14 +12364,17 @@
       </c>
       <c r="DZ35" s="0">
         <v>144.456</v>
+      </c>
+      <c r="EA35" s="0">
+        <v>145.463</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C36" s="0">
         <v>42.37</v>
@@ -12665,14 +12759,17 @@
       </c>
       <c r="DZ36" s="0">
         <v>143.256</v>
+      </c>
+      <c r="EA36" s="0">
+        <v>144.398</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C37" s="0">
         <v>37.917</v>
@@ -13057,14 +13154,17 @@
       </c>
       <c r="DZ37" s="0">
         <v>136.122</v>
+      </c>
+      <c r="EA37" s="0">
+        <v>136.514</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" s="0">
         <v>45.901</v>
@@ -13449,14 +13549,17 @@
       </c>
       <c r="DZ38" s="0">
         <v>149.546</v>
+      </c>
+      <c r="EA38" s="0">
+        <v>151.401</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C39" s="0">
         <v>326.427</v>
@@ -13841,64 +13944,67 @@
       </c>
       <c r="DZ39" s="0">
         <v>94.587</v>
+      </c>
+      <c r="EA39" s="0">
+        <v>94.011</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:DZ1"/>
-    <mergeCell ref="A2:DZ2"/>
-    <mergeCell ref="A3:DZ3"/>
-    <mergeCell ref="A4:DZ4"/>
+    <mergeCell ref="A1:EA1"/>
+    <mergeCell ref="A2:EA2"/>
+    <mergeCell ref="A3:EA3"/>
+    <mergeCell ref="A4:EA4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:F6"/>
@@ -13933,16 +14039,16 @@
     <mergeCell ref="DO6:DR6"/>
     <mergeCell ref="DS6:DV6"/>
     <mergeCell ref="DW6:DZ6"/>
-    <mergeCell ref="A40:EA40"/>
-    <mergeCell ref="A41:EA41"/>
-    <mergeCell ref="A42:EA42"/>
-    <mergeCell ref="A43:EA43"/>
-    <mergeCell ref="A44:EA44"/>
-    <mergeCell ref="A45:EA45"/>
-    <mergeCell ref="A46:EA46"/>
-    <mergeCell ref="A47:EA47"/>
-    <mergeCell ref="A48:EA48"/>
-    <mergeCell ref="A49:EA49"/>
+    <mergeCell ref="A40:EB40"/>
+    <mergeCell ref="A41:EB41"/>
+    <mergeCell ref="A42:EB42"/>
+    <mergeCell ref="A43:EB43"/>
+    <mergeCell ref="A44:EB44"/>
+    <mergeCell ref="A45:EB45"/>
+    <mergeCell ref="A46:EB46"/>
+    <mergeCell ref="A47:EB47"/>
+    <mergeCell ref="A48:EB48"/>
+    <mergeCell ref="A49:EB49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>